<commit_message>
continuing to work on LOLCat webpage
</commit_message>
<xml_diff>
--- a/Study Timesheet.xlsx
+++ b/Study Timesheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19100" windowHeight="7270"/>
+    <workbookView windowWidth="19100" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22">
   <si>
     <t>Study time sheet</t>
   </si>
@@ -44,6 +44,42 @@
   </si>
   <si>
     <t>Monday</t>
+  </si>
+  <si>
+    <t>Continuing React/ trying to successfully run JSX</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>React tutorial with Mosh Hamedani</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Went back to basics - working on LOL Cat Clock - from scratch on my own. // practiced fonts/width. Also closely looked at pixels and my screen is 1280 horizontally.</t>
+  </si>
+  <si>
+    <t>Continued practice with LOLCat</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Restarted working on LOL Cat - Finally started back up after the initial Craziness. * Had bug in where h4 and h4 span was displaing all clumped up in same line. Fix was that in Css I had to manually specify h4 and h4 #(spand id name). //because if i don't make this distinction in CSS all will be clumped up in H4. *** Also another bug was when indicating margin-top i did not place px at end to indicate pixels.</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Work on conecting the clock a.k.a JavaScript</t>
+  </si>
+  <si>
+    <t>Working on iteration part of clock and whole project, maybe inserting pics and switch opterations today??? // Once again reLearned how to use the debugging tool, it's inspect element and then console, if errors then look for the line number. *** In this case I misspelled a var and was useing wrong var names thereafter so this was bug. I used var  minuets = ...   //misspelled minutes *** // Fluent in all 3 steps now, css and js both functions.</t>
+  </si>
+  <si>
+    <t>Thursday</t>
   </si>
 </sst>
 </file>
@@ -51,13 +87,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="h:mm;@"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="h:mm;@"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="180" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -76,6 +112,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -83,11 +181,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -101,113 +199,51 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,36 +265,102 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -271,7 +373,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,103 +385,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,24 +446,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,6 +470,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -464,15 +509,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,13 +561,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -543,40 +579,40 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -585,88 +621,88 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -686,16 +722,16 @@
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1019,18 +1055,21 @@
   <sheetPr/>
   <dimension ref="A2:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26.1818181818182" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.18181818181818"/>
+    <col min="2" max="2" width="10.2727272727273"/>
     <col min="3" max="3" width="18.8181818181818" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.45454545454546"/>
+    <col min="4" max="5" width="9.45454545454546"/>
+    <col min="6" max="6" width="9.27272727272727"/>
     <col min="8" max="8" width="9.45454545454546"/>
+    <col min="9" max="9" width="9.27272727272727"/>
     <col min="10" max="10" width="18.0909090909091" customWidth="1"/>
+    <col min="11" max="11" width="26.3636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" ht="31" spans="4:4">
@@ -1125,69 +1164,137 @@
         <v>0.277777777777778</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+    <row r="7" ht="29" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6">
+        <v>43929</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.986111111111111</v>
+      </c>
+      <c r="E7" s="5">
+        <v>43930.0319444444</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.0451388888888889</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.0951388888888889</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="8" t="str">
-        <f t="shared" ref="J7:J14" si="0">IF(D7,(E7-D7)+(G7-F7)+(I7-H7),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="6"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="J7" s="8">
+        <f t="shared" ref="J7:J15" si="0">IF(D7,(E7-D7)+(G7-F7)+(I7-H7),"")</f>
+        <v>43929.0958333333</v>
+      </c>
+    </row>
+    <row r="8" ht="29" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="6">
+        <v>43931</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.692361111111111</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.742361111111111</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="8" t="str">
+      <c r="J8" s="8">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="6"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" ht="29" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6">
+        <v>43932</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5">
+        <v>43932.9819444444</v>
+      </c>
+      <c r="E9" s="5">
+        <v>43933.1875</v>
+      </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="8" t="str">
+      <c r="J9" s="8">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="6"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+        <v>0.205555555599858</v>
+      </c>
+    </row>
+    <row r="10" ht="87" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="6">
+        <v>43938</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.740277777777778</v>
+      </c>
+      <c r="E10" s="5">
+        <v>43938.8388888889</v>
+      </c>
+      <c r="F10" s="5">
+        <v>43939.0888888889</v>
+      </c>
+      <c r="G10" s="5">
+        <v>43939.2145833333</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="8" t="str">
+      <c r="J10" s="8">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="6"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+        <v>43938.2243055555</v>
+      </c>
+    </row>
+    <row r="11" ht="29" spans="1:10">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="6">
+        <v>43939</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="5">
+        <v>43939.0319444444</v>
+      </c>
+      <c r="E11" s="5">
+        <v>43940.0875</v>
+      </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="8" t="str">
+      <c r="J11" s="8">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1.0555555555984</v>
       </c>
     </row>
     <row r="12" spans="2:10">
@@ -1203,40 +1310,100 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="6"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="8" t="str">
+    <row r="13" ht="217.5" spans="1:10">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="6">
+        <v>44061</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.597916666666667</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.611111111111111</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.638888888888889</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.68125</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="J13" s="8">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="6"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+        <v>0.0972222222222223</v>
+      </c>
+    </row>
+    <row r="14" ht="29" spans="1:10">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="6">
+        <v>44062</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.635416666666667</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.684027777777778</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.702777777777778</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.741666666666667</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="8" t="str">
+      <c r="J14" s="8">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="2:9">
-      <c r="B15" s="6"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+        <v>0.0875000000000001</v>
+      </c>
+    </row>
+    <row r="15" ht="232" spans="1:10">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="6">
+        <v>44063</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.517361111111111</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.600694444444444</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.868055555555556</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0.923611111111111</v>
+      </c>
+      <c r="J15" s="8">
+        <f t="shared" si="0"/>
+        <v>0.201388888888889</v>
+      </c>
     </row>
     <row r="16" spans="2:9">
       <c r="B16" s="6"/>

</xml_diff>